<commit_message>
fixes for paper submission
</commit_message>
<xml_diff>
--- a/annotation/Single cell studies database-Specifics.xlsx
+++ b/annotation/Single cell studies database-Specifics.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saskiafreytag/Desktop/Neuronal_Maturation/neuro_mat/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A8A9E8-76B6-394C-B203-306B2CC9F9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF65550-337C-4548-83A5-2786C35A65F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="2760" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{400F3A48-CB5E-407D-8322-D41CC6BAEF8D}"/>
+    <workbookView xWindow="6840" yWindow="500" windowWidth="28800" windowHeight="16360" activeTab="1" xr2:uid="{400F3A48-CB5E-407D-8322-D41CC6BAEF8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Fetal" sheetId="8" r:id="rId1"/>
-    <sheet name="Postnatal" sheetId="9" r:id="rId2"/>
-    <sheet name="Nowakowski" sheetId="1" r:id="rId3"/>
-    <sheet name="Darmanis" sheetId="2" r:id="rId4"/>
-    <sheet name="Lake NBT" sheetId="3" r:id="rId5"/>
-    <sheet name="Jakel" sheetId="4" r:id="rId6"/>
-    <sheet name="Mathys" sheetId="5" r:id="rId7"/>
-    <sheet name="Velmeshev" sheetId="6" r:id="rId8"/>
-    <sheet name="Schirmer" sheetId="7" r:id="rId9"/>
+    <sheet name="ATAC" sheetId="10" r:id="rId2"/>
+    <sheet name="Postnatal" sheetId="9" r:id="rId3"/>
+    <sheet name="Nowakowski" sheetId="1" r:id="rId4"/>
+    <sheet name="Darmanis" sheetId="2" r:id="rId5"/>
+    <sheet name="Lake NBT" sheetId="3" r:id="rId6"/>
+    <sheet name="Jakel" sheetId="4" r:id="rId7"/>
+    <sheet name="Mathys" sheetId="5" r:id="rId8"/>
+    <sheet name="Velmeshev" sheetId="6" r:id="rId9"/>
+    <sheet name="Schirmer" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Lake NBT'!$A$1:$J$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Lake NBT'!$A$1:$J$56</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2787" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2963" uniqueCount="369">
   <si>
     <t>Name</t>
   </si>
@@ -1108,6 +1109,42 @@
   <si>
     <t>18-79</t>
   </si>
+  <si>
+    <t>Trevino</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Eze</t>
+  </si>
+  <si>
+    <t>Study</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Fetal</t>
+  </si>
+  <si>
+    <t>sci-ATAC-seq3</t>
+  </si>
+  <si>
+    <t>Domcke</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Pfister</t>
+  </si>
+  <si>
+    <t>Corces</t>
+  </si>
 </sst>
 </file>
 
@@ -1116,7 +1153,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1350,6 +1387,19 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1D1C1D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1928,7 +1978,7 @@
     <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2109,6 +2159,9 @@
     <xf numFmtId="1" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2145,6 +2198,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="20% - Accent1 2" xfId="26" xr:uid="{CAE76D19-A6E4-4248-BE53-46B37DC05F6D}"/>
@@ -2555,10 +2609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66400606-65AC-4192-92B4-AC9BBE339EEC}">
-  <dimension ref="A1:E140"/>
+  <dimension ref="A1:E158"/>
   <sheetViews>
-    <sheetView topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141:C157"/>
+    <sheetView topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4945,18 +4999,1947 @@
         <v>354</v>
       </c>
     </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B141" s="49">
+        <v>16</v>
+      </c>
+      <c r="C141" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D141" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E141" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B142" s="49">
+        <v>16</v>
+      </c>
+      <c r="C142" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D142" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E142" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B143" s="49">
+        <v>20</v>
+      </c>
+      <c r="C143" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D143" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E143" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B144" s="49">
+        <v>20</v>
+      </c>
+      <c r="C144" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D144" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E144" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B145" s="49">
+        <v>21</v>
+      </c>
+      <c r="C145" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D145" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E145" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B146" s="49">
+        <v>21</v>
+      </c>
+      <c r="C146" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D146" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E146" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B147" s="49">
+        <v>24</v>
+      </c>
+      <c r="C147" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D147" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E147" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B148" s="49">
+        <v>24</v>
+      </c>
+      <c r="C148" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D148" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E148" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" s="49" t="s">
+        <v>359</v>
+      </c>
+      <c r="B149" s="49">
+        <v>22</v>
+      </c>
+      <c r="C149" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D149" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E149" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" s="49" t="s">
+        <v>359</v>
+      </c>
+      <c r="B150" s="49">
+        <v>22</v>
+      </c>
+      <c r="C150" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D150" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E150" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" s="49" t="s">
+        <v>359</v>
+      </c>
+      <c r="B151" s="49">
+        <v>20</v>
+      </c>
+      <c r="C151" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D151" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E151" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" s="49" t="s">
+        <v>359</v>
+      </c>
+      <c r="B152" s="49">
+        <v>19</v>
+      </c>
+      <c r="C152" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D152" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E152" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" s="49" t="s">
+        <v>359</v>
+      </c>
+      <c r="B153" s="49">
+        <v>15</v>
+      </c>
+      <c r="C153" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D153" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E153" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" s="49" t="s">
+        <v>359</v>
+      </c>
+      <c r="B154" s="49">
+        <v>15</v>
+      </c>
+      <c r="C154" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D154" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E154" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" s="49" t="s">
+        <v>359</v>
+      </c>
+      <c r="B155" s="49">
+        <v>14</v>
+      </c>
+      <c r="C155" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D155" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E155" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" s="49" t="s">
+        <v>359</v>
+      </c>
+      <c r="B156" s="49">
+        <v>14</v>
+      </c>
+      <c r="C156" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D156" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E156" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" s="49" t="s">
+        <v>359</v>
+      </c>
+      <c r="B157" s="49">
+        <v>13</v>
+      </c>
+      <c r="C157" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D157" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E157" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" s="49" t="s">
+        <v>359</v>
+      </c>
+      <c r="B158" s="49">
+        <v>12</v>
+      </c>
+      <c r="C158" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D158" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E158" s="49" t="s">
+        <v>354</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E813DD09-AF27-4276-B62F-BB556B33C644}">
+  <dimension ref="A1:O24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" activeCellId="1" sqref="A4:A12 K4:K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="75" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="77" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>240</v>
+      </c>
+      <c r="I1" s="73" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="73" t="s">
+        <v>241</v>
+      </c>
+      <c r="K1" s="73" t="s">
+        <v>230</v>
+      </c>
+      <c r="L1" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="M1" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="N1" s="73" t="s">
+        <v>242</v>
+      </c>
+      <c r="O1" s="71" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="75"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="71"/>
+    </row>
+    <row r="3" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="76"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="72"/>
+    </row>
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>245</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>246</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="H4" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="I4" s="42">
+        <v>21</v>
+      </c>
+      <c r="J4" s="42">
+        <v>8.5</v>
+      </c>
+      <c r="K4" s="42">
+        <v>82</v>
+      </c>
+      <c r="L4" s="42" t="s">
+        <v>247</v>
+      </c>
+      <c r="M4" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="N4" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="O4" s="44">
+        <v>0.54900000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="42" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="H5" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="I5" s="42">
+        <v>15</v>
+      </c>
+      <c r="J5" s="42">
+        <v>7.3</v>
+      </c>
+      <c r="K5" s="42">
+        <v>61</v>
+      </c>
+      <c r="L5" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="M5" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="N5" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="O5" s="44">
+        <v>0.42099999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="I6" s="42">
+        <v>18</v>
+      </c>
+      <c r="J6" s="42">
+        <v>7.5</v>
+      </c>
+      <c r="K6" s="42">
+        <v>64</v>
+      </c>
+      <c r="L6" s="42" t="s">
+        <v>247</v>
+      </c>
+      <c r="M6" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="N6" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="O6" s="44">
+        <v>0.65900000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="42" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="H7" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="I7" s="42">
+        <v>30</v>
+      </c>
+      <c r="J7" s="42">
+        <v>8.5</v>
+      </c>
+      <c r="K7" s="42">
+        <v>68</v>
+      </c>
+      <c r="L7" s="42" t="s">
+        <v>247</v>
+      </c>
+      <c r="M7" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="N7" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="O7" s="44">
+        <v>0.71899999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>260</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="H8" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="I8" s="42">
+        <v>22</v>
+      </c>
+      <c r="J8" s="42">
+        <v>6.8</v>
+      </c>
+      <c r="K8" s="42">
+        <v>35</v>
+      </c>
+      <c r="L8" s="42" t="s">
+        <v>247</v>
+      </c>
+      <c r="M8" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="N8" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="O8" s="44">
+        <v>0.84299999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="42" t="s">
+        <v>261</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="H9" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="I9" s="42">
+        <v>27</v>
+      </c>
+      <c r="J9" s="42">
+        <v>7.4</v>
+      </c>
+      <c r="K9" s="42">
+        <v>34</v>
+      </c>
+      <c r="L9" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="M9" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="N9" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="O9" s="44">
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="42" t="s">
+        <v>263</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="H10" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="I10" s="42">
+        <v>16</v>
+      </c>
+      <c r="J10" s="42">
+        <v>7.5</v>
+      </c>
+      <c r="K10" s="42">
+        <v>39</v>
+      </c>
+      <c r="L10" s="42" t="s">
+        <v>247</v>
+      </c>
+      <c r="M10" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="N10" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="O10" s="44">
+        <v>0.64500000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="42" t="s">
+        <v>265</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>266</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="G11" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="H11" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="I11" s="42">
+        <v>19</v>
+      </c>
+      <c r="J11" s="42">
+        <v>7.1</v>
+      </c>
+      <c r="K11" s="42">
+        <v>44</v>
+      </c>
+      <c r="L11" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="M11" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="N11" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="O11" s="44">
+        <v>0.71299999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="42" t="s">
+        <v>267</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>268</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="I12" s="42">
+        <v>6</v>
+      </c>
+      <c r="J12" s="42">
+        <v>8.5</v>
+      </c>
+      <c r="K12" s="42">
+        <v>54</v>
+      </c>
+      <c r="L12" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="M12" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="N12" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="O12" s="44">
+        <v>0.45400000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="39" t="s">
+        <v>269</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>254</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="F13" s="40">
+        <v>26</v>
+      </c>
+      <c r="G13" s="40">
+        <v>7</v>
+      </c>
+      <c r="H13" s="40">
+        <v>28</v>
+      </c>
+      <c r="I13" s="39">
+        <v>9</v>
+      </c>
+      <c r="J13" s="39">
+        <v>7</v>
+      </c>
+      <c r="K13" s="39">
+        <v>35</v>
+      </c>
+      <c r="L13" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="M13" s="39">
+        <v>5</v>
+      </c>
+      <c r="N13" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="O13" s="41">
+        <v>0.67100000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>273</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>274</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="F14" s="40">
+        <v>51</v>
+      </c>
+      <c r="G14" s="40">
+        <v>20</v>
+      </c>
+      <c r="H14" s="40">
+        <v>62</v>
+      </c>
+      <c r="I14" s="39">
+        <v>22</v>
+      </c>
+      <c r="J14" s="39">
+        <v>8.9</v>
+      </c>
+      <c r="K14" s="39">
+        <v>50</v>
+      </c>
+      <c r="L14" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="M14" s="39">
+        <v>23</v>
+      </c>
+      <c r="N14" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="O14" s="41">
+        <v>0.67799999999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+      <c r="A15" s="39" t="s">
+        <v>275</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>277</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>260</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="F15" s="40">
+        <v>26</v>
+      </c>
+      <c r="G15" s="40">
+        <v>17</v>
+      </c>
+      <c r="H15" s="40">
+        <v>38</v>
+      </c>
+      <c r="I15" s="39">
+        <v>10</v>
+      </c>
+      <c r="J15" s="39">
+        <v>9</v>
+      </c>
+      <c r="K15" s="39">
+        <v>51</v>
+      </c>
+      <c r="L15" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="M15" s="39">
+        <v>23</v>
+      </c>
+      <c r="N15" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="O15" s="41">
+        <v>0.46899999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>279</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>251</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="F16" s="40">
+        <v>40</v>
+      </c>
+      <c r="G16" s="40">
+        <v>16</v>
+      </c>
+      <c r="H16" s="40">
+        <v>38</v>
+      </c>
+      <c r="I16" s="39">
+        <v>11</v>
+      </c>
+      <c r="J16" s="39">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="K16" s="39">
+        <v>42</v>
+      </c>
+      <c r="L16" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="M16" s="39">
+        <v>6</v>
+      </c>
+      <c r="N16" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="O16" s="41">
+        <v>0.66800000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>283</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>260</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="F17" s="40">
+        <v>12</v>
+      </c>
+      <c r="G17" s="40">
+        <v>6</v>
+      </c>
+      <c r="H17" s="40">
+        <v>11</v>
+      </c>
+      <c r="I17" s="39">
+        <v>12</v>
+      </c>
+      <c r="J17" s="39">
+        <v>8.9</v>
+      </c>
+      <c r="K17" s="39">
+        <v>34</v>
+      </c>
+      <c r="L17" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="M17" s="39">
+        <v>11</v>
+      </c>
+      <c r="N17" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="O17" s="41">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="39" t="s">
+        <v>284</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>251</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="F18" s="40">
+        <v>30</v>
+      </c>
+      <c r="G18" s="40">
+        <v>9</v>
+      </c>
+      <c r="H18" s="40">
+        <v>43</v>
+      </c>
+      <c r="I18" s="39">
+        <v>27</v>
+      </c>
+      <c r="J18" s="39">
+        <v>7.9</v>
+      </c>
+      <c r="K18" s="39">
+        <v>40</v>
+      </c>
+      <c r="L18" s="39" t="s">
+        <v>247</v>
+      </c>
+      <c r="M18" s="39">
+        <v>16</v>
+      </c>
+      <c r="N18" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="O18" s="41">
+        <v>0.753</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="39" t="s">
+        <v>287</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>288</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>251</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="F19" s="40">
+        <v>49</v>
+      </c>
+      <c r="G19" s="40">
+        <v>33</v>
+      </c>
+      <c r="H19" s="40">
+        <v>93</v>
+      </c>
+      <c r="I19" s="39">
+        <v>27</v>
+      </c>
+      <c r="J19" s="39">
+        <v>7.6</v>
+      </c>
+      <c r="K19" s="39">
+        <v>40</v>
+      </c>
+      <c r="L19" s="39" t="s">
+        <v>247</v>
+      </c>
+      <c r="M19" s="39">
+        <v>16</v>
+      </c>
+      <c r="N19" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="O19" s="41">
+        <v>0.57799999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="39" t="s">
+        <v>289</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>273</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>290</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>251</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="F20" s="40">
+        <v>32</v>
+      </c>
+      <c r="G20" s="40">
+        <v>7</v>
+      </c>
+      <c r="H20" s="40">
+        <v>67</v>
+      </c>
+      <c r="I20" s="39">
+        <v>22</v>
+      </c>
+      <c r="J20" s="39">
+        <v>8.9</v>
+      </c>
+      <c r="K20" s="39">
+        <v>50</v>
+      </c>
+      <c r="L20" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="M20" s="39">
+        <v>23</v>
+      </c>
+      <c r="N20" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="O20" s="41">
+        <v>0.68200000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" s="39" t="s">
+        <v>291</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>292</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>260</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>294</v>
+      </c>
+      <c r="F21" s="40">
+        <v>64</v>
+      </c>
+      <c r="G21" s="40">
+        <v>21</v>
+      </c>
+      <c r="H21" s="40">
+        <v>42</v>
+      </c>
+      <c r="I21" s="39">
+        <v>16</v>
+      </c>
+      <c r="J21" s="39">
+        <v>7.1</v>
+      </c>
+      <c r="K21" s="39">
+        <v>55</v>
+      </c>
+      <c r="L21" s="39" t="s">
+        <v>247</v>
+      </c>
+      <c r="M21" s="39">
+        <v>43</v>
+      </c>
+      <c r="N21" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="O21" s="41">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+      <c r="A22" s="39" t="s">
+        <v>295</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="D22" s="40" t="s">
+        <v>260</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>294</v>
+      </c>
+      <c r="F22" s="40">
+        <v>31</v>
+      </c>
+      <c r="G22" s="40">
+        <v>7</v>
+      </c>
+      <c r="H22" s="40">
+        <v>46</v>
+      </c>
+      <c r="I22" s="39">
+        <v>13</v>
+      </c>
+      <c r="J22" s="39">
+        <v>7</v>
+      </c>
+      <c r="K22" s="39">
+        <v>53</v>
+      </c>
+      <c r="L22" s="39" t="s">
+        <v>247</v>
+      </c>
+      <c r="M22" s="39">
+        <v>16</v>
+      </c>
+      <c r="N22" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="O22" s="41">
+        <v>0.54400000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" s="39" t="s">
+        <v>298</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>260</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>294</v>
+      </c>
+      <c r="F23" s="40">
+        <v>23</v>
+      </c>
+      <c r="G23" s="40">
+        <v>6</v>
+      </c>
+      <c r="H23" s="40">
+        <v>23</v>
+      </c>
+      <c r="I23" s="39">
+        <v>21</v>
+      </c>
+      <c r="J23" s="39">
+        <v>9.1</v>
+      </c>
+      <c r="K23" s="39">
+        <v>48</v>
+      </c>
+      <c r="L23" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="M23" s="39">
+        <v>29</v>
+      </c>
+      <c r="N23" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="O23" s="41">
+        <v>0.41599999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="39" t="s">
+        <v>301</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>251</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>294</v>
+      </c>
+      <c r="F24" s="40">
+        <v>41</v>
+      </c>
+      <c r="G24" s="40">
+        <v>6</v>
+      </c>
+      <c r="H24" s="40">
+        <v>12</v>
+      </c>
+      <c r="I24" s="39">
+        <v>20</v>
+      </c>
+      <c r="J24" s="39">
+        <v>9</v>
+      </c>
+      <c r="K24" s="39">
+        <v>44</v>
+      </c>
+      <c r="L24" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="M24" s="39">
+        <v>19</v>
+      </c>
+      <c r="N24" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="O24" s="41">
+        <v>0.70799999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="N1:N3"/>
+    <mergeCell ref="J1:J3"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="M1:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF8CC3D-3557-A248-80D3-747F1A51EFA7}">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B2" s="66">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>363</v>
+      </c>
+      <c r="D2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B3" s="66">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>364</v>
+      </c>
+      <c r="B4" s="66">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D4" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>364</v>
+      </c>
+      <c r="B5" s="66">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>363</v>
+      </c>
+      <c r="D5" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>364</v>
+      </c>
+      <c r="B6" s="66">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>363</v>
+      </c>
+      <c r="D6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>364</v>
+      </c>
+      <c r="B7" s="66">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D7" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>364</v>
+      </c>
+      <c r="B8" s="66">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>363</v>
+      </c>
+      <c r="D8" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>364</v>
+      </c>
+      <c r="B9" s="66">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>363</v>
+      </c>
+      <c r="D9" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>364</v>
+      </c>
+      <c r="B10" s="66">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>363</v>
+      </c>
+      <c r="D10" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>364</v>
+      </c>
+      <c r="B11" s="66">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>363</v>
+      </c>
+      <c r="D11" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="79" t="s">
+        <v>368</v>
+      </c>
+      <c r="B12" s="66">
+        <v>86</v>
+      </c>
+      <c r="C12" t="s">
+        <v>327</v>
+      </c>
+      <c r="D12" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="79" t="s">
+        <v>368</v>
+      </c>
+      <c r="B13" s="66">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>327</v>
+      </c>
+      <c r="D13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="79" t="s">
+        <v>368</v>
+      </c>
+      <c r="B14" s="66">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>327</v>
+      </c>
+      <c r="D14" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="79" t="s">
+        <v>368</v>
+      </c>
+      <c r="B15" s="66">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>327</v>
+      </c>
+      <c r="D15" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="79" t="s">
+        <v>368</v>
+      </c>
+      <c r="B16" s="66">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
+        <v>327</v>
+      </c>
+      <c r="D16" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="79" t="s">
+        <v>368</v>
+      </c>
+      <c r="B17" s="66">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>327</v>
+      </c>
+      <c r="D17" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="79" t="s">
+        <v>368</v>
+      </c>
+      <c r="B18" s="66">
+        <v>88</v>
+      </c>
+      <c r="C18" t="s">
+        <v>327</v>
+      </c>
+      <c r="D18" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="79" t="s">
+        <v>368</v>
+      </c>
+      <c r="B19" s="66">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s">
+        <v>327</v>
+      </c>
+      <c r="D19" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="79" t="s">
+        <v>368</v>
+      </c>
+      <c r="B20" s="66">
+        <v>91</v>
+      </c>
+      <c r="C20" t="s">
+        <v>327</v>
+      </c>
+      <c r="D20" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="79" t="s">
+        <v>368</v>
+      </c>
+      <c r="B21" s="66">
+        <v>95</v>
+      </c>
+      <c r="C21" t="s">
+        <v>327</v>
+      </c>
+      <c r="D21" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B22" s="49">
+        <v>16</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D22" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B23" s="49">
+        <v>16</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D23" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B24" s="49">
+        <v>20</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D24" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B25" s="49">
+        <v>20</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D25" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B26" s="49">
+        <v>21</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D26" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B27" s="49">
+        <v>21</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D27" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B28" s="49">
+        <v>24</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D28" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="49" t="s">
+        <v>352</v>
+      </c>
+      <c r="B29">
+        <v>79</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D29" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="49" t="s">
+        <v>352</v>
+      </c>
+      <c r="B30">
+        <v>90</v>
+      </c>
+      <c r="C30" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D30" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="49" t="s">
+        <v>352</v>
+      </c>
+      <c r="B31">
+        <v>74</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D31" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="49" t="s">
+        <v>352</v>
+      </c>
+      <c r="B32">
+        <v>83</v>
+      </c>
+      <c r="C32" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D32" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="49" t="s">
+        <v>352</v>
+      </c>
+      <c r="B33">
+        <v>90</v>
+      </c>
+      <c r="C33" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D33" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="49" t="s">
+        <v>352</v>
+      </c>
+      <c r="B34">
+        <v>79</v>
+      </c>
+      <c r="C34" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D34" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="49" t="s">
+        <v>352</v>
+      </c>
+      <c r="B35">
+        <v>79</v>
+      </c>
+      <c r="C35" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D35" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="49" t="s">
+        <v>352</v>
+      </c>
+      <c r="B36">
+        <v>79</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D36" t="s">
+        <v>366</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="32" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8B34-A02D-4375-8594-463A9315FFB5}">
-  <dimension ref="A1:F200"/>
+  <dimension ref="A1:G199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="I197" sqref="I197"/>
+    <sheetView topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7462,7 +9445,7 @@
     </row>
     <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="54" t="s">
-        <v>304</v>
+        <v>367</v>
       </c>
       <c r="B127" s="52">
         <v>22</v>
@@ -7482,7 +9465,7 @@
     </row>
     <row r="128" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="54" t="s">
-        <v>304</v>
+        <v>367</v>
       </c>
       <c r="B128" s="52">
         <v>34</v>
@@ -7502,7 +9485,7 @@
     </row>
     <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="54" t="s">
-        <v>304</v>
+        <v>367</v>
       </c>
       <c r="B129" s="52">
         <v>39</v>
@@ -7522,7 +9505,7 @@
     </row>
     <row r="130" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="54" t="s">
-        <v>304</v>
+        <v>367</v>
       </c>
       <c r="B130" s="52">
         <v>44</v>
@@ -7542,7 +9525,7 @@
     </row>
     <row r="131" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="54" t="s">
-        <v>304</v>
+        <v>367</v>
       </c>
       <c r="B131" s="52">
         <v>54</v>
@@ -8460,7 +10443,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" s="60" t="s">
         <v>352</v>
       </c>
@@ -8480,12 +10463,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" s="60" t="s">
         <v>352</v>
       </c>
       <c r="B178" s="59">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C178" s="60" t="s">
         <v>327</v>
@@ -8500,12 +10483,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" s="60" t="s">
         <v>352</v>
       </c>
       <c r="B179" s="59">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C179" s="60" t="s">
         <v>327</v>
@@ -8520,12 +10503,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="60" t="s">
         <v>352</v>
       </c>
       <c r="B180" s="59">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C180" s="60" t="s">
         <v>327</v>
@@ -8540,7 +10523,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" s="60" t="s">
         <v>352</v>
       </c>
@@ -8560,7 +10543,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" s="60" t="s">
         <v>352</v>
       </c>
@@ -8580,12 +10563,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" s="60" t="s">
-        <v>352</v>
-      </c>
-      <c r="B183" s="59">
-        <v>79</v>
+        <v>355</v>
+      </c>
+      <c r="B183" s="59" t="s">
+        <v>356</v>
       </c>
       <c r="C183" s="60" t="s">
         <v>327</v>
@@ -8599,8 +10582,11 @@
       <c r="F183" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G183" s="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="60" t="s">
         <v>355</v>
       </c>
@@ -8619,8 +10605,11 @@
       <c r="F184" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G184" s="60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="60" t="s">
         <v>355</v>
       </c>
@@ -8639,8 +10628,11 @@
       <c r="F185" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G185" s="60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" s="60" t="s">
         <v>355</v>
       </c>
@@ -8659,8 +10651,11 @@
       <c r="F186" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G186" s="60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" s="60" t="s">
         <v>355</v>
       </c>
@@ -8679,8 +10674,11 @@
       <c r="F187" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G187" s="60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="60" t="s">
         <v>355</v>
       </c>
@@ -8699,8 +10697,11 @@
       <c r="F188" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G188" s="60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" s="60" t="s">
         <v>355</v>
       </c>
@@ -8719,8 +10720,11 @@
       <c r="F189" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G189" s="60">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="60" t="s">
         <v>355</v>
       </c>
@@ -8739,8 +10743,11 @@
       <c r="F190" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G190" s="60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" s="60" t="s">
         <v>355</v>
       </c>
@@ -8759,8 +10766,11 @@
       <c r="F191" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G191" s="60">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" s="60" t="s">
         <v>355</v>
       </c>
@@ -8779,8 +10789,11 @@
       <c r="F192" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G192" s="60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" s="60" t="s">
         <v>355</v>
       </c>
@@ -8799,8 +10812,11 @@
       <c r="F193" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G193" s="60">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" s="60" t="s">
         <v>355</v>
       </c>
@@ -8819,8 +10835,11 @@
       <c r="F194" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G194" s="60">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" s="60" t="s">
         <v>355</v>
       </c>
@@ -8839,8 +10858,11 @@
       <c r="F195" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G195" s="60">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" s="60" t="s">
         <v>355</v>
       </c>
@@ -8859,8 +10881,11 @@
       <c r="F196" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G196" s="60">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" s="60" t="s">
         <v>355</v>
       </c>
@@ -8879,8 +10904,11 @@
       <c r="F197" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G197" s="60">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" s="60" t="s">
         <v>355</v>
       </c>
@@ -8899,8 +10927,11 @@
       <c r="F198" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G198" s="60">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" s="60" t="s">
         <v>355</v>
       </c>
@@ -8919,25 +10950,8 @@
       <c r="F199" s="60" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A200" s="60" t="s">
-        <v>355</v>
-      </c>
-      <c r="B200" s="59" t="s">
-        <v>356</v>
-      </c>
-      <c r="C200" s="60" t="s">
-        <v>327</v>
-      </c>
-      <c r="D200" s="60" t="s">
-        <v>328</v>
-      </c>
-      <c r="E200" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="F200" s="60" t="s">
-        <v>99</v>
+      <c r="G199" s="60">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -8950,7 +10964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5016DA3-0E88-40CB-9D2E-132C65F3E86B}">
   <dimension ref="A1:E4262"/>
   <sheetViews>
@@ -39299,7 +41313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D7824F-0B3A-44F6-90B9-388DB1B2458C}">
   <dimension ref="L2"/>
   <sheetViews>
@@ -39323,7 +41337,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD894B98-82D4-4E5F-96DD-5B09018FC155}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J56"/>
@@ -41120,7 +43134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DA8193-62E3-4B9F-8131-7B357E6D082E}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -41159,12 +43173,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="67" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="69"/>
       <c r="E2" s="8" t="s">
         <v>142</v>
       </c>
@@ -41360,7 +43374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28628DC6-3D63-4D56-985F-3CE5D3E5EFD4}">
   <dimension ref="A1:J49"/>
   <sheetViews>
@@ -42943,7 +44957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61DE9DB0-A9C6-4E44-A674-AD251B4C94DD}">
   <dimension ref="A1:K48"/>
   <sheetViews>
@@ -42966,28 +44980,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="70" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="70" t="s">
         <v>229</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="70" t="s">
         <v>230</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="70" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="70" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
       <c r="G2" s="37" t="s">
         <v>228</v>
       </c>
@@ -44084,1107 +46098,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E813DD09-AF27-4276-B62F-BB556B33C644}">
-  <dimension ref="A1:O24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" activeCellId="1" sqref="A4:A12 K4:K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="74" t="s">
-        <v>233</v>
-      </c>
-      <c r="B1" s="76" t="s">
-        <v>234</v>
-      </c>
-      <c r="C1" s="72" t="s">
-        <v>235</v>
-      </c>
-      <c r="D1" s="72" t="s">
-        <v>236</v>
-      </c>
-      <c r="E1" s="72" t="s">
-        <v>237</v>
-      </c>
-      <c r="F1" s="72" t="s">
-        <v>238</v>
-      </c>
-      <c r="G1" s="72" t="s">
-        <v>239</v>
-      </c>
-      <c r="H1" s="72" t="s">
-        <v>240</v>
-      </c>
-      <c r="I1" s="72" t="s">
-        <v>94</v>
-      </c>
-      <c r="J1" s="72" t="s">
-        <v>241</v>
-      </c>
-      <c r="K1" s="72" t="s">
-        <v>230</v>
-      </c>
-      <c r="L1" s="72" t="s">
-        <v>136</v>
-      </c>
-      <c r="M1" s="72" t="s">
-        <v>140</v>
-      </c>
-      <c r="N1" s="72" t="s">
-        <v>242</v>
-      </c>
-      <c r="O1" s="70" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="74"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="70"/>
-    </row>
-    <row r="3" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75"/>
-      <c r="B3" s="77"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="71"/>
-    </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
-        <v>244</v>
-      </c>
-      <c r="B4" s="43" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>245</v>
-      </c>
-      <c r="D4" s="43" t="s">
-        <v>246</v>
-      </c>
-      <c r="E4" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F4" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="G4" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="H4" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="I4" s="42">
-        <v>21</v>
-      </c>
-      <c r="J4" s="42">
-        <v>8.5</v>
-      </c>
-      <c r="K4" s="42">
-        <v>82</v>
-      </c>
-      <c r="L4" s="42" t="s">
-        <v>247</v>
-      </c>
-      <c r="M4" s="42" t="s">
-        <v>155</v>
-      </c>
-      <c r="N4" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="O4" s="44">
-        <v>0.54900000000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
-        <v>248</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>249</v>
-      </c>
-      <c r="C5" s="43" t="s">
-        <v>250</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="G5" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="H5" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="I5" s="42">
-        <v>15</v>
-      </c>
-      <c r="J5" s="42">
-        <v>7.3</v>
-      </c>
-      <c r="K5" s="42">
-        <v>61</v>
-      </c>
-      <c r="L5" s="42" t="s">
-        <v>252</v>
-      </c>
-      <c r="M5" s="42" t="s">
-        <v>155</v>
-      </c>
-      <c r="N5" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="O5" s="44">
-        <v>0.42099999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
-        <v>253</v>
-      </c>
-      <c r="B6" s="43" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>254</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>246</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="G6" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="H6" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="I6" s="42">
-        <v>18</v>
-      </c>
-      <c r="J6" s="42">
-        <v>7.5</v>
-      </c>
-      <c r="K6" s="42">
-        <v>64</v>
-      </c>
-      <c r="L6" s="42" t="s">
-        <v>247</v>
-      </c>
-      <c r="M6" s="42" t="s">
-        <v>155</v>
-      </c>
-      <c r="N6" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="O6" s="44">
-        <v>0.65900000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="42" t="s">
-        <v>255</v>
-      </c>
-      <c r="B7" s="43" t="s">
-        <v>256</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>257</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="E7" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F7" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="G7" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="H7" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="I7" s="42">
-        <v>30</v>
-      </c>
-      <c r="J7" s="42">
-        <v>8.5</v>
-      </c>
-      <c r="K7" s="42">
-        <v>68</v>
-      </c>
-      <c r="L7" s="42" t="s">
-        <v>247</v>
-      </c>
-      <c r="M7" s="42" t="s">
-        <v>155</v>
-      </c>
-      <c r="N7" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="O7" s="44">
-        <v>0.71899999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="42" t="s">
-        <v>258</v>
-      </c>
-      <c r="B8" s="43" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>259</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>260</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F8" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="G8" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="H8" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="I8" s="42">
-        <v>22</v>
-      </c>
-      <c r="J8" s="42">
-        <v>6.8</v>
-      </c>
-      <c r="K8" s="42">
-        <v>35</v>
-      </c>
-      <c r="L8" s="42" t="s">
-        <v>247</v>
-      </c>
-      <c r="M8" s="42" t="s">
-        <v>155</v>
-      </c>
-      <c r="N8" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="O8" s="44">
-        <v>0.84299999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="42" t="s">
-        <v>261</v>
-      </c>
-      <c r="B9" s="43" t="s">
-        <v>262</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="G9" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="H9" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="I9" s="42">
-        <v>27</v>
-      </c>
-      <c r="J9" s="42">
-        <v>7.4</v>
-      </c>
-      <c r="K9" s="42">
-        <v>34</v>
-      </c>
-      <c r="L9" s="42" t="s">
-        <v>252</v>
-      </c>
-      <c r="M9" s="42" t="s">
-        <v>155</v>
-      </c>
-      <c r="N9" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="O9" s="44">
-        <v>0.72799999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
-        <v>263</v>
-      </c>
-      <c r="B10" s="43" t="s">
-        <v>264</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="E10" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="G10" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="H10" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="I10" s="42">
-        <v>16</v>
-      </c>
-      <c r="J10" s="42">
-        <v>7.5</v>
-      </c>
-      <c r="K10" s="42">
-        <v>39</v>
-      </c>
-      <c r="L10" s="42" t="s">
-        <v>247</v>
-      </c>
-      <c r="M10" s="42" t="s">
-        <v>155</v>
-      </c>
-      <c r="N10" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="O10" s="44">
-        <v>0.64500000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="42" t="s">
-        <v>265</v>
-      </c>
-      <c r="B11" s="43" t="s">
-        <v>266</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="E11" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="G11" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="H11" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="I11" s="42">
-        <v>19</v>
-      </c>
-      <c r="J11" s="42">
-        <v>7.1</v>
-      </c>
-      <c r="K11" s="42">
-        <v>44</v>
-      </c>
-      <c r="L11" s="42" t="s">
-        <v>252</v>
-      </c>
-      <c r="M11" s="42" t="s">
-        <v>155</v>
-      </c>
-      <c r="N11" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="O11" s="44">
-        <v>0.71299999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="42" t="s">
-        <v>267</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>268</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D12" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F12" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="G12" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="H12" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="I12" s="42">
-        <v>6</v>
-      </c>
-      <c r="J12" s="42">
-        <v>8.5</v>
-      </c>
-      <c r="K12" s="42">
-        <v>54</v>
-      </c>
-      <c r="L12" s="42" t="s">
-        <v>252</v>
-      </c>
-      <c r="M12" s="42" t="s">
-        <v>155</v>
-      </c>
-      <c r="N12" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="O12" s="44">
-        <v>0.45400000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="39" t="s">
-        <v>269</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>270</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>254</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="F13" s="40">
-        <v>26</v>
-      </c>
-      <c r="G13" s="40">
-        <v>7</v>
-      </c>
-      <c r="H13" s="40">
-        <v>28</v>
-      </c>
-      <c r="I13" s="39">
-        <v>9</v>
-      </c>
-      <c r="J13" s="39">
-        <v>7</v>
-      </c>
-      <c r="K13" s="39">
-        <v>35</v>
-      </c>
-      <c r="L13" s="39" t="s">
-        <v>252</v>
-      </c>
-      <c r="M13" s="39">
-        <v>5</v>
-      </c>
-      <c r="N13" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="O13" s="41">
-        <v>0.67100000000000004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="39" t="s">
-        <v>272</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>273</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>274</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="F14" s="40">
-        <v>51</v>
-      </c>
-      <c r="G14" s="40">
-        <v>20</v>
-      </c>
-      <c r="H14" s="40">
-        <v>62</v>
-      </c>
-      <c r="I14" s="39">
-        <v>22</v>
-      </c>
-      <c r="J14" s="39">
-        <v>8.9</v>
-      </c>
-      <c r="K14" s="39">
-        <v>50</v>
-      </c>
-      <c r="L14" s="39" t="s">
-        <v>252</v>
-      </c>
-      <c r="M14" s="39">
-        <v>23</v>
-      </c>
-      <c r="N14" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="O14" s="41">
-        <v>0.67799999999999994</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="39" t="s">
-        <v>275</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>276</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>277</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>260</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="F15" s="40">
-        <v>26</v>
-      </c>
-      <c r="G15" s="40">
-        <v>17</v>
-      </c>
-      <c r="H15" s="40">
-        <v>38</v>
-      </c>
-      <c r="I15" s="39">
-        <v>10</v>
-      </c>
-      <c r="J15" s="39">
-        <v>9</v>
-      </c>
-      <c r="K15" s="39">
-        <v>51</v>
-      </c>
-      <c r="L15" s="39" t="s">
-        <v>252</v>
-      </c>
-      <c r="M15" s="39">
-        <v>23</v>
-      </c>
-      <c r="N15" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="O15" s="41">
-        <v>0.46899999999999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="B16" s="40" t="s">
-        <v>279</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>280</v>
-      </c>
-      <c r="D16" s="40" t="s">
-        <v>251</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="F16" s="40">
-        <v>40</v>
-      </c>
-      <c r="G16" s="40">
-        <v>16</v>
-      </c>
-      <c r="H16" s="40">
-        <v>38</v>
-      </c>
-      <c r="I16" s="39">
-        <v>11</v>
-      </c>
-      <c r="J16" s="39">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="K16" s="39">
-        <v>42</v>
-      </c>
-      <c r="L16" s="39" t="s">
-        <v>252</v>
-      </c>
-      <c r="M16" s="39">
-        <v>6</v>
-      </c>
-      <c r="N16" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="O16" s="41">
-        <v>0.66800000000000004</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="39" t="s">
-        <v>281</v>
-      </c>
-      <c r="B17" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>283</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>260</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="F17" s="40">
-        <v>12</v>
-      </c>
-      <c r="G17" s="40">
-        <v>6</v>
-      </c>
-      <c r="H17" s="40">
-        <v>11</v>
-      </c>
-      <c r="I17" s="39">
-        <v>12</v>
-      </c>
-      <c r="J17" s="39">
-        <v>8.9</v>
-      </c>
-      <c r="K17" s="39">
-        <v>34</v>
-      </c>
-      <c r="L17" s="39" t="s">
-        <v>252</v>
-      </c>
-      <c r="M17" s="39">
-        <v>11</v>
-      </c>
-      <c r="N17" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="O17" s="41">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="39" t="s">
-        <v>284</v>
-      </c>
-      <c r="B18" s="40" t="s">
-        <v>285</v>
-      </c>
-      <c r="C18" s="40" t="s">
-        <v>286</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>251</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="F18" s="40">
-        <v>30</v>
-      </c>
-      <c r="G18" s="40">
-        <v>9</v>
-      </c>
-      <c r="H18" s="40">
-        <v>43</v>
-      </c>
-      <c r="I18" s="39">
-        <v>27</v>
-      </c>
-      <c r="J18" s="39">
-        <v>7.9</v>
-      </c>
-      <c r="K18" s="39">
-        <v>40</v>
-      </c>
-      <c r="L18" s="39" t="s">
-        <v>247</v>
-      </c>
-      <c r="M18" s="39">
-        <v>16</v>
-      </c>
-      <c r="N18" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="O18" s="41">
-        <v>0.753</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="39" t="s">
-        <v>287</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>285</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>288</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>251</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="F19" s="40">
-        <v>49</v>
-      </c>
-      <c r="G19" s="40">
-        <v>33</v>
-      </c>
-      <c r="H19" s="40">
-        <v>93</v>
-      </c>
-      <c r="I19" s="39">
-        <v>27</v>
-      </c>
-      <c r="J19" s="39">
-        <v>7.6</v>
-      </c>
-      <c r="K19" s="39">
-        <v>40</v>
-      </c>
-      <c r="L19" s="39" t="s">
-        <v>247</v>
-      </c>
-      <c r="M19" s="39">
-        <v>16</v>
-      </c>
-      <c r="N19" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="O19" s="41">
-        <v>0.57799999999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="39" t="s">
-        <v>289</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>273</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>290</v>
-      </c>
-      <c r="D20" s="40" t="s">
-        <v>251</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>271</v>
-      </c>
-      <c r="F20" s="40">
-        <v>32</v>
-      </c>
-      <c r="G20" s="40">
-        <v>7</v>
-      </c>
-      <c r="H20" s="40">
-        <v>67</v>
-      </c>
-      <c r="I20" s="39">
-        <v>22</v>
-      </c>
-      <c r="J20" s="39">
-        <v>8.9</v>
-      </c>
-      <c r="K20" s="39">
-        <v>50</v>
-      </c>
-      <c r="L20" s="39" t="s">
-        <v>252</v>
-      </c>
-      <c r="M20" s="39">
-        <v>23</v>
-      </c>
-      <c r="N20" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="O20" s="41">
-        <v>0.68200000000000005</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="39" t="s">
-        <v>291</v>
-      </c>
-      <c r="B21" s="40" t="s">
-        <v>292</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>293</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>260</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>294</v>
-      </c>
-      <c r="F21" s="40">
-        <v>64</v>
-      </c>
-      <c r="G21" s="40">
-        <v>21</v>
-      </c>
-      <c r="H21" s="40">
-        <v>42</v>
-      </c>
-      <c r="I21" s="39">
-        <v>16</v>
-      </c>
-      <c r="J21" s="39">
-        <v>7.1</v>
-      </c>
-      <c r="K21" s="39">
-        <v>55</v>
-      </c>
-      <c r="L21" s="39" t="s">
-        <v>247</v>
-      </c>
-      <c r="M21" s="39">
-        <v>43</v>
-      </c>
-      <c r="N21" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="O21" s="41">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.2">
-      <c r="A22" s="39" t="s">
-        <v>295</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>296</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>297</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>260</v>
-      </c>
-      <c r="E22" s="39" t="s">
-        <v>294</v>
-      </c>
-      <c r="F22" s="40">
-        <v>31</v>
-      </c>
-      <c r="G22" s="40">
-        <v>7</v>
-      </c>
-      <c r="H22" s="40">
-        <v>46</v>
-      </c>
-      <c r="I22" s="39">
-        <v>13</v>
-      </c>
-      <c r="J22" s="39">
-        <v>7</v>
-      </c>
-      <c r="K22" s="39">
-        <v>53</v>
-      </c>
-      <c r="L22" s="39" t="s">
-        <v>247</v>
-      </c>
-      <c r="M22" s="39">
-        <v>16</v>
-      </c>
-      <c r="N22" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="O22" s="41">
-        <v>0.54400000000000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" s="39" t="s">
-        <v>298</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>299</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>300</v>
-      </c>
-      <c r="D23" s="40" t="s">
-        <v>260</v>
-      </c>
-      <c r="E23" s="39" t="s">
-        <v>294</v>
-      </c>
-      <c r="F23" s="40">
-        <v>23</v>
-      </c>
-      <c r="G23" s="40">
-        <v>6</v>
-      </c>
-      <c r="H23" s="40">
-        <v>23</v>
-      </c>
-      <c r="I23" s="39">
-        <v>21</v>
-      </c>
-      <c r="J23" s="39">
-        <v>9.1</v>
-      </c>
-      <c r="K23" s="39">
-        <v>48</v>
-      </c>
-      <c r="L23" s="39" t="s">
-        <v>252</v>
-      </c>
-      <c r="M23" s="39">
-        <v>29</v>
-      </c>
-      <c r="N23" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="O23" s="41">
-        <v>0.41599999999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="39" t="s">
-        <v>301</v>
-      </c>
-      <c r="B24" s="40" t="s">
-        <v>302</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>286</v>
-      </c>
-      <c r="D24" s="40" t="s">
-        <v>251</v>
-      </c>
-      <c r="E24" s="39" t="s">
-        <v>294</v>
-      </c>
-      <c r="F24" s="40">
-        <v>41</v>
-      </c>
-      <c r="G24" s="40">
-        <v>6</v>
-      </c>
-      <c r="H24" s="40">
-        <v>12</v>
-      </c>
-      <c r="I24" s="39">
-        <v>20</v>
-      </c>
-      <c r="J24" s="39">
-        <v>9</v>
-      </c>
-      <c r="K24" s="39">
-        <v>44</v>
-      </c>
-      <c r="L24" s="39" t="s">
-        <v>252</v>
-      </c>
-      <c r="M24" s="39">
-        <v>19</v>
-      </c>
-      <c r="N24" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="O24" s="41">
-        <v>0.70799999999999996</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="N1:N3"/>
-    <mergeCell ref="J1:J3"/>
-    <mergeCell ref="K1:K3"/>
-    <mergeCell ref="L1:L3"/>
-    <mergeCell ref="M1:M3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add Saskia snRNA code
</commit_message>
<xml_diff>
--- a/annotation/Single cell studies database-Specifics.xlsx
+++ b/annotation/Single cell studies database-Specifics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saskiafreytag/Desktop/Neuronal_Maturation/neuro_mat/annotation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/freytag.s/Desktop/neuronal_mat/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF65550-337C-4548-83A5-2786C35A65F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCBC4A1-D87B-4044-8380-9930E24BE3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="500" windowWidth="28800" windowHeight="16360" activeTab="1" xr2:uid="{400F3A48-CB5E-407D-8322-D41CC6BAEF8D}"/>
+    <workbookView xWindow="9600" yWindow="500" windowWidth="28800" windowHeight="16360" activeTab="2" xr2:uid="{400F3A48-CB5E-407D-8322-D41CC6BAEF8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Fetal" sheetId="8" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2963" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3068" uniqueCount="379">
   <si>
     <t>Name</t>
   </si>
@@ -1145,6 +1145,36 @@
   <si>
     <t>Corces</t>
   </si>
+  <si>
+    <t>Yang</t>
+  </si>
+  <si>
+    <t>MFC</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Caudate</t>
+  </si>
+  <si>
+    <t>Caudate/Put</t>
+  </si>
+  <si>
+    <t>Kamath</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>Luo</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>snmCAT-seq</t>
+  </si>
 </sst>
 </file>
 
@@ -1153,7 +1183,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1404,8 +1434,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1615,8 +1651,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1926,6 +1968,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1978,7 +2035,7 @@
     <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2162,6 +2219,17 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -2198,7 +2266,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="20% - Accent1 2" xfId="26" xr:uid="{CAE76D19-A6E4-4248-BE53-46B37DC05F6D}"/>
@@ -5325,85 +5392,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="80" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="82" t="s">
         <v>234</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="78" t="s">
         <v>235</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="78" t="s">
         <v>236</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="78" t="s">
         <v>237</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="78" t="s">
         <v>238</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="78" t="s">
         <v>239</v>
       </c>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="78" t="s">
         <v>240</v>
       </c>
-      <c r="I1" s="73" t="s">
+      <c r="I1" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="73" t="s">
+      <c r="J1" s="78" t="s">
         <v>241</v>
       </c>
-      <c r="K1" s="73" t="s">
+      <c r="K1" s="78" t="s">
         <v>230</v>
       </c>
-      <c r="L1" s="73" t="s">
+      <c r="L1" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="M1" s="73" t="s">
+      <c r="M1" s="78" t="s">
         <v>140</v>
       </c>
-      <c r="N1" s="73" t="s">
+      <c r="N1" s="78" t="s">
         <v>242</v>
       </c>
-      <c r="O1" s="71" t="s">
+      <c r="O1" s="76" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="75"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="71"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="76"/>
     </row>
     <row r="3" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="72"/>
+      <c r="A3" s="81"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="77"/>
     </row>
     <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
@@ -6418,7 +6485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF8CC3D-3557-A248-80D3-747F1A51EFA7}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -6579,7 +6646,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="79" t="s">
+      <c r="A12" s="67" t="s">
         <v>368</v>
       </c>
       <c r="B12" s="66">
@@ -6593,7 +6660,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="67" t="s">
         <v>368</v>
       </c>
       <c r="B13" s="66">
@@ -6607,7 +6674,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="67" t="s">
         <v>368</v>
       </c>
       <c r="B14" s="66">
@@ -6621,7 +6688,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="79" t="s">
+      <c r="A15" s="67" t="s">
         <v>368</v>
       </c>
       <c r="B15" s="66">
@@ -6635,7 +6702,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="79" t="s">
+      <c r="A16" s="67" t="s">
         <v>368</v>
       </c>
       <c r="B16" s="66">
@@ -6649,7 +6716,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="79" t="s">
+      <c r="A17" s="67" t="s">
         <v>368</v>
       </c>
       <c r="B17" s="66">
@@ -6663,7 +6730,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="79" t="s">
+      <c r="A18" s="67" t="s">
         <v>368</v>
       </c>
       <c r="B18" s="66">
@@ -6677,7 +6744,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="67" t="s">
         <v>368</v>
       </c>
       <c r="B19" s="66">
@@ -6691,7 +6758,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="79" t="s">
+      <c r="A20" s="67" t="s">
         <v>368</v>
       </c>
       <c r="B20" s="66">
@@ -6705,7 +6772,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="79" t="s">
+      <c r="A21" s="67" t="s">
         <v>368</v>
       </c>
       <c r="B21" s="66">
@@ -6936,10 +7003,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8B34-A02D-4375-8594-463A9315FFB5}">
-  <dimension ref="A1:G199"/>
+  <dimension ref="A1:G220"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="L211" sqref="L211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10952,6 +11019,426 @@
       </c>
       <c r="G199" s="60">
         <v>17</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A200" s="60" t="s">
+        <v>369</v>
+      </c>
+      <c r="B200" s="68">
+        <v>71</v>
+      </c>
+      <c r="C200" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D200" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E200" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="F200" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A201" s="60" t="s">
+        <v>369</v>
+      </c>
+      <c r="B201" s="69">
+        <v>82</v>
+      </c>
+      <c r="C201" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D201" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E201" s="60" t="s">
+        <v>370</v>
+      </c>
+      <c r="F201" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A202" s="60" t="s">
+        <v>369</v>
+      </c>
+      <c r="B202" s="69">
+        <v>77</v>
+      </c>
+      <c r="C202" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D202" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E202" s="60" t="s">
+        <v>370</v>
+      </c>
+      <c r="F202" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A203" s="60" t="s">
+        <v>369</v>
+      </c>
+      <c r="B203" s="68">
+        <v>90</v>
+      </c>
+      <c r="C203" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D203" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E203" s="60" t="s">
+        <v>370</v>
+      </c>
+      <c r="F203" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A204" s="60" t="s">
+        <v>369</v>
+      </c>
+      <c r="B204" s="69">
+        <v>83</v>
+      </c>
+      <c r="C204" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D204" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E204" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="F204" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A205" s="60" t="s">
+        <v>369</v>
+      </c>
+      <c r="B205" s="68">
+        <v>63</v>
+      </c>
+      <c r="C205" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D205" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E205" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="F205" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A206" s="60" t="s">
+        <v>371</v>
+      </c>
+      <c r="B206" s="68">
+        <v>82</v>
+      </c>
+      <c r="C206" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D206" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E206" s="60" t="s">
+        <v>372</v>
+      </c>
+      <c r="F206" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A207" s="60" t="s">
+        <v>371</v>
+      </c>
+      <c r="B207" s="59">
+        <v>80</v>
+      </c>
+      <c r="C207" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D207" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E207" s="60" t="s">
+        <v>373</v>
+      </c>
+      <c r="F207" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A208" s="60" t="s">
+        <v>371</v>
+      </c>
+      <c r="B208" s="59">
+        <v>70</v>
+      </c>
+      <c r="C208" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D208" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E208" s="60" t="s">
+        <v>373</v>
+      </c>
+      <c r="F208" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A209" s="60" t="s">
+        <v>371</v>
+      </c>
+      <c r="B209" s="59">
+        <v>67</v>
+      </c>
+      <c r="C209" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D209" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E209" s="60" t="s">
+        <v>373</v>
+      </c>
+      <c r="F209" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A210" s="60" t="s">
+        <v>371</v>
+      </c>
+      <c r="B210" s="59">
+        <v>83</v>
+      </c>
+      <c r="C210" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D210" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E210" s="60" t="s">
+        <v>372</v>
+      </c>
+      <c r="F210" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A211" s="70" t="s">
+        <v>374</v>
+      </c>
+      <c r="B211" s="71">
+        <v>90</v>
+      </c>
+      <c r="C211" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D211" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E211" s="60" t="s">
+        <v>375</v>
+      </c>
+      <c r="F211" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A212" s="70" t="s">
+        <v>374</v>
+      </c>
+      <c r="B212" s="71">
+        <v>79</v>
+      </c>
+      <c r="C212" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D212" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E212" s="60" t="s">
+        <v>375</v>
+      </c>
+      <c r="F212" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A213" s="70" t="s">
+        <v>374</v>
+      </c>
+      <c r="B213" s="71">
+        <v>92</v>
+      </c>
+      <c r="C213" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D213" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E213" s="60" t="s">
+        <v>375</v>
+      </c>
+      <c r="F213" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A214" s="70" t="s">
+        <v>374</v>
+      </c>
+      <c r="B214" s="71">
+        <v>82</v>
+      </c>
+      <c r="C214" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D214" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E214" s="60" t="s">
+        <v>375</v>
+      </c>
+      <c r="F214" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A215" s="70" t="s">
+        <v>374</v>
+      </c>
+      <c r="B215" s="71">
+        <v>79</v>
+      </c>
+      <c r="C215" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D215" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E215" s="60" t="s">
+        <v>375</v>
+      </c>
+      <c r="F215" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A216" s="70" t="s">
+        <v>374</v>
+      </c>
+      <c r="B216" s="71">
+        <v>91</v>
+      </c>
+      <c r="C216" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D216" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E216" s="60" t="s">
+        <v>375</v>
+      </c>
+      <c r="F216" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A217" s="70" t="s">
+        <v>374</v>
+      </c>
+      <c r="B217" s="71">
+        <v>49</v>
+      </c>
+      <c r="C217" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D217" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E217" s="60" t="s">
+        <v>375</v>
+      </c>
+      <c r="F217" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A218" s="70" t="s">
+        <v>374</v>
+      </c>
+      <c r="B218" s="71">
+        <v>50</v>
+      </c>
+      <c r="C218" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="D218" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E218" s="60" t="s">
+        <v>375</v>
+      </c>
+      <c r="F218" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A219" s="60" t="s">
+        <v>376</v>
+      </c>
+      <c r="B219" s="59">
+        <v>21</v>
+      </c>
+      <c r="C219" s="60" t="s">
+        <v>378</v>
+      </c>
+      <c r="D219" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E219" s="60" t="s">
+        <v>377</v>
+      </c>
+      <c r="F219" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A220" s="60" t="s">
+        <v>376</v>
+      </c>
+      <c r="B220" s="59">
+        <v>29</v>
+      </c>
+      <c r="C220" s="60" t="s">
+        <v>378</v>
+      </c>
+      <c r="D220" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="E220" s="60" t="s">
+        <v>377</v>
+      </c>
+      <c r="F220" s="60" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -43173,12 +43660,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="72" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="69"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="74"/>
       <c r="E2" s="8" t="s">
         <v>142</v>
       </c>
@@ -44980,28 +45467,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="75" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="75" t="s">
         <v>229</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="75" t="s">
         <v>230</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="75" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="75" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
       <c r="G2" s="37" t="s">
         <v>228</v>
       </c>

</xml_diff>